<commit_message>
First data wrangling of chemical analysis data set.
</commit_message>
<xml_diff>
--- a/volatiles.xlsx
+++ b/volatiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Documents\Github\first_year_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851F3D51-F391-4D88-8C71-D4DE1B975780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D30A4EF-5797-4842-88A0-5397D8265C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05C1D990-8F4B-4A40-A91B-DB847C5D4403}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>